<commit_message>
19/06/23　Reduce.hs : findliveを実装中
</commit_message>
<xml_diff>
--- a/callGraph.xlsx
+++ b/callGraph.xlsx
@@ -11,13 +11,14 @@
     <sheet name="ver1" sheetId="2" r:id="rId2"/>
     <sheet name="ver1作業シート" sheetId="3" r:id="rId3"/>
     <sheet name="ver2" sheetId="4" r:id="rId4"/>
+    <sheet name="ver2作業シート" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9040" uniqueCount="2141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9050" uniqueCount="2151">
   <si>
     <t>CheckSymmetry</t>
     <phoneticPr fontId="1"/>
@@ -8765,6 +8766,429 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> :: TpConfmat -&gt; [Bool] -&gt; Bool -&gt; Int -&gt; Bool</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>power</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>findliveSubSub2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :: [Int] -&gt; [Int] -&gt; Int -&gt; Int -&gt; Int</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>printStatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :: Int -&gt; Int -&gt; Int -&gt; Int -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ()</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>findliveSubSubSub</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :: Int -&gt; Int -&gt; Int -&gt; TpFindlivePack -&gt; Int -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ContT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TpFindlivePack </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TpFindlivePack</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>findliveSubSub1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :: Int -&gt; Int -&gt; Int -&gt; TpFindlivePack -&gt; Int -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ContT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TpFindlivePack </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TpFindlivePack</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>findlive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :: [Int] -&gt; Int -&gt; TpAngle -&gt; [Int] -&gt; Int -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Int, [Int])</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>findliveSub</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :: Int -&gt; TpAngle -&gt; [Int] -&gt; Int -&gt; Int -&gt; Int -&gt; TpFindlivePack -&gt; Int -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ContT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TpFindlivePack </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TpFindlivePack</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>record</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :: [Int] -&gt; [Int] -&gt; Int -&gt; TpAngle -&gt; [Int] -&gt; Int -&gt; Int -&gt; (Int, [Int])</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>recordSub1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :: [Int] -&gt; [Int] -&gt; TpAngle -&gt; [Int] -&gt; Int -&gt; [Int]</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>recordSub2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :: [Int] -&gt; (Int, Int) -&gt; Int -&gt; (Int, Int)</t>
     </r>
     <phoneticPr fontId="1"/>
   </si>
@@ -40138,10 +40562,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L115"/>
+  <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -40873,9 +41297,54 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="115" spans="7:7">
+    <row r="115" spans="5:8">
       <c r="G115" s="2" t="s">
         <v>2140</v>
+      </c>
+    </row>
+    <row r="119" spans="5:8">
+      <c r="E119" s="2" t="s">
+        <v>2146</v>
+      </c>
+    </row>
+    <row r="120" spans="5:8">
+      <c r="F120" s="2" t="s">
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="121" spans="5:8">
+      <c r="G121" s="2" t="s">
+        <v>2148</v>
+      </c>
+    </row>
+    <row r="122" spans="5:8">
+      <c r="H122" s="2" t="s">
+        <v>2149</v>
+      </c>
+    </row>
+    <row r="125" spans="5:8">
+      <c r="H125" s="2" t="s">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="128" spans="5:8">
+      <c r="G128" s="2" t="s">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="131" spans="7:9">
+      <c r="G131" s="2" t="s">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="132" spans="7:9">
+      <c r="H132" s="2" t="s">
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="133" spans="7:9">
+      <c r="I133" s="2" t="s">
+        <v>2143</v>
       </c>
     </row>
   </sheetData>
@@ -40883,4 +41352,170 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="3" max="3" width="13.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="C3" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>3^(B4-1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f>3^(B5-1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C19" si="0">3^(B6-1)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>729</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>6561</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>19683</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>59049</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>177147</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>531441</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1594323</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>4782969</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>14348907</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>